<commit_message>
updated format of larval daily measurements sheet
</commit_message>
<xml_diff>
--- a/data/environmental/daily_measurements/larval_daily_measurements.xlsx
+++ b/data/environmental/daily_measurements/larval_daily_measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hputnam/MyProjects/apulchra_metabolism/data/environmental/daily_measurements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianasnowhuffmyer/MyProjects/E5/apulchra_metabolism/data/environmental/daily_measurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151B7C5B-82BD-6149-937B-42DAAFFD429D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96CC46F-8C6F-2440-BA1F-728180924DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="1900" windowWidth="27640" windowHeight="16440" xr2:uid="{06FF1615-EDFC-CC40-A177-C5790F94CB7B}"/>
+    <workbookView xWindow="-35340" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{06FF1615-EDFC-CC40-A177-C5790F94CB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -51,27 +51,9 @@
     <t>sal.psu</t>
   </si>
   <si>
-    <t>flow.mL.5s.initial</t>
-  </si>
-  <si>
-    <t>flow.mL.5s.final</t>
-  </si>
-  <si>
     <t>par.center</t>
   </si>
   <si>
-    <t>par.q1</t>
-  </si>
-  <si>
-    <t>par.q2</t>
-  </si>
-  <si>
-    <t>par.q3</t>
-  </si>
-  <si>
-    <t>par.q4</t>
-  </si>
-  <si>
     <t>tris.date</t>
   </si>
   <si>
@@ -100,6 +82,9 @@
   </si>
   <si>
     <t>cloudy, rainy</t>
+  </si>
+  <si>
+    <t>flow.mL.5s</t>
   </si>
 </sst>
 </file>
@@ -453,15 +438,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E9C5AE7-F5F9-8844-8420-93F51018B107}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,34 +469,19 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44847</v>
       </c>
@@ -516,7 +489,7 @@
         <v>0.45277777777777778</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>27.44</v>
@@ -528,31 +501,16 @@
         <v>38.14</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>441</v>
       </c>
       <c r="I2">
-        <v>441</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2">
-        <v>20220924</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <v>20220924</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44847</v>
       </c>
@@ -560,7 +518,7 @@
         <v>0.45416666666666666</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>27.54</v>
@@ -572,31 +530,16 @@
         <v>38.14</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>455</v>
       </c>
       <c r="I3">
-        <v>455</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3">
-        <v>20220924</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <v>20220924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44847</v>
       </c>
@@ -604,7 +547,7 @@
         <v>0.45555555555555555</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>27.63</v>
@@ -616,31 +559,16 @@
         <v>38.15</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>453</v>
       </c>
       <c r="I4">
-        <v>453</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4">
-        <v>20220924</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>20220924</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44847</v>
       </c>
@@ -648,7 +576,7 @@
         <v>0.45694444444444443</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>28.06</v>
@@ -660,31 +588,16 @@
         <v>38.15</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>480</v>
       </c>
       <c r="I5">
-        <v>480</v>
-      </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5">
-        <v>20220924</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>20220924</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44848</v>
       </c>
@@ -692,7 +605,7 @@
         <v>0.43958333333333338</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>27.82</v>
@@ -704,34 +617,19 @@
         <v>38.08</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>329</v>
       </c>
       <c r="I6">
-        <v>329</v>
+        <v>20220924</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6">
-        <v>20220924</v>
-      </c>
-      <c r="O6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44848</v>
       </c>
@@ -739,7 +637,7 @@
         <v>0.44097222222222227</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>27.78</v>
@@ -751,34 +649,19 @@
         <v>38.1</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>333</v>
       </c>
       <c r="I7">
-        <v>333</v>
+        <v>20220924</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7">
-        <v>20220924</v>
-      </c>
-      <c r="O7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44848</v>
       </c>
@@ -786,7 +669,7 @@
         <v>0.44166666666666665</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>27.88</v>
@@ -798,34 +681,19 @@
         <v>38.14</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>350</v>
       </c>
       <c r="I8">
-        <v>350</v>
+        <v>20220924</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8">
-        <v>20220924</v>
-      </c>
-      <c r="O8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44848</v>
       </c>
@@ -833,7 +701,7 @@
         <v>0.44236111111111115</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>28.54</v>
@@ -845,34 +713,19 @@
         <v>38.159999999999997</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>393</v>
       </c>
       <c r="I9">
-        <v>393</v>
+        <v>20220924</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" t="s">
-        <v>16</v>
-      </c>
-      <c r="N9">
-        <v>20220924</v>
-      </c>
-      <c r="O9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44849</v>
       </c>
@@ -880,7 +733,7 @@
         <v>0.60625000000000007</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>27.92</v>
@@ -892,34 +745,19 @@
         <v>38.19</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>372</v>
       </c>
       <c r="I10">
-        <v>372</v>
+        <v>20220924</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N10">
-        <v>20220924</v>
-      </c>
-      <c r="O10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44849</v>
       </c>
@@ -927,7 +765,7 @@
         <v>0.6069444444444444</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D11">
         <v>28.01</v>
@@ -939,34 +777,19 @@
         <v>38.159999999999997</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>338</v>
       </c>
       <c r="I11">
-        <v>338</v>
+        <v>20220924</v>
       </c>
       <c r="J11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11">
-        <v>20220924</v>
-      </c>
-      <c r="O11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44849</v>
       </c>
@@ -974,7 +797,7 @@
         <v>0.60763888888888895</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D12">
         <v>27.93</v>
@@ -986,34 +809,19 @@
         <v>38.18</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>334</v>
       </c>
       <c r="I12">
-        <v>334</v>
+        <v>20220924</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12">
-        <v>20220924</v>
-      </c>
-      <c r="O12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44849</v>
       </c>
@@ -1021,7 +829,7 @@
         <v>0.60833333333333328</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D13">
         <v>27.84</v>
@@ -1033,34 +841,19 @@
         <v>38.130000000000003</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>382</v>
       </c>
       <c r="I13">
-        <v>382</v>
+        <v>20220924</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13" t="s">
-        <v>16</v>
-      </c>
-      <c r="N13">
-        <v>20220924</v>
-      </c>
-      <c r="O13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44850</v>
       </c>
@@ -1068,7 +861,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <v>27.86</v>
@@ -1080,31 +873,16 @@
         <v>38.090000000000003</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>203</v>
       </c>
       <c r="I14">
-        <v>203</v>
-      </c>
-      <c r="J14" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14" t="s">
-        <v>16</v>
-      </c>
-      <c r="N14">
-        <v>20220924</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>20220924</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44850</v>
       </c>
@@ -1112,7 +890,7 @@
         <v>0.58402777777777781</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D15">
         <v>27.83</v>
@@ -1124,31 +902,16 @@
         <v>38.17</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>189</v>
       </c>
       <c r="I15">
-        <v>189</v>
-      </c>
-      <c r="J15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L15" t="s">
-        <v>16</v>
-      </c>
-      <c r="M15" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15">
-        <v>20220924</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <v>20220924</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44850</v>
       </c>
@@ -1156,7 +919,7 @@
         <v>0.58472222222222225</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D16">
         <v>27.79</v>
@@ -1168,31 +931,16 @@
         <v>38.19</v>
       </c>
       <c r="G16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>197</v>
       </c>
       <c r="I16">
-        <v>197</v>
-      </c>
-      <c r="J16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N16">
-        <v>20220924</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+        <v>20220924</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44850</v>
       </c>
@@ -1200,7 +948,7 @@
         <v>0.5854166666666667</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>27.82</v>
@@ -1212,31 +960,16 @@
         <v>38.200000000000003</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>214</v>
       </c>
       <c r="I17">
-        <v>214</v>
-      </c>
-      <c r="J17" t="s">
-        <v>16</v>
-      </c>
-      <c r="K17" t="s">
-        <v>16</v>
-      </c>
-      <c r="L17" t="s">
-        <v>16</v>
-      </c>
-      <c r="M17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N17">
-        <v>20220924</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+        <v>20220924</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44851</v>
       </c>
@@ -1244,7 +977,7 @@
         <v>0.53819444444444442</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D18">
         <v>27.76</v>
@@ -1256,34 +989,19 @@
         <v>38.21</v>
       </c>
       <c r="G18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>185</v>
       </c>
       <c r="I18">
-        <v>185</v>
+        <v>20220924</v>
       </c>
       <c r="J18" t="s">
         <v>16</v>
       </c>
-      <c r="K18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L18" t="s">
-        <v>16</v>
-      </c>
-      <c r="M18" t="s">
-        <v>16</v>
-      </c>
-      <c r="N18">
-        <v>20220924</v>
-      </c>
-      <c r="O18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44851</v>
       </c>
@@ -1291,7 +1009,7 @@
         <v>0.5395833333333333</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D19">
         <v>27.73</v>
@@ -1303,34 +1021,19 @@
         <v>38.200000000000003</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>193</v>
       </c>
       <c r="I19">
-        <v>193</v>
+        <v>20220924</v>
       </c>
       <c r="J19" t="s">
         <v>16</v>
       </c>
-      <c r="K19" t="s">
-        <v>16</v>
-      </c>
-      <c r="L19" t="s">
-        <v>16</v>
-      </c>
-      <c r="M19" t="s">
-        <v>16</v>
-      </c>
-      <c r="N19">
-        <v>20220924</v>
-      </c>
-      <c r="O19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44851</v>
       </c>
@@ -1338,7 +1041,7 @@
         <v>0.54027777777777775</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D20">
         <v>27.75</v>
@@ -1350,34 +1053,19 @@
         <v>38.200000000000003</v>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>179</v>
       </c>
       <c r="I20">
-        <v>179</v>
+        <v>20220924</v>
       </c>
       <c r="J20" t="s">
         <v>16</v>
       </c>
-      <c r="K20" t="s">
-        <v>16</v>
-      </c>
-      <c r="L20" t="s">
-        <v>16</v>
-      </c>
-      <c r="M20" t="s">
-        <v>16</v>
-      </c>
-      <c r="N20">
-        <v>20220924</v>
-      </c>
-      <c r="O20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44851</v>
       </c>
@@ -1385,7 +1073,7 @@
         <v>0.54097222222222219</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D21">
         <v>27.76</v>
@@ -1397,31 +1085,16 @@
         <v>38.21</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>258</v>
       </c>
       <c r="I21">
-        <v>258</v>
+        <v>20220924</v>
       </c>
       <c r="J21" t="s">
         <v>16</v>
-      </c>
-      <c r="K21" t="s">
-        <v>16</v>
-      </c>
-      <c r="L21" t="s">
-        <v>16</v>
-      </c>
-      <c r="M21" t="s">
-        <v>16</v>
-      </c>
-      <c r="N21">
-        <v>20220924</v>
-      </c>
-      <c r="O21" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>